<commit_message>
US_TO_EXPOSURE_VALUE, EXPOSURE_VALUE_TO_US, TO_VOLTAGE_OUT helper macros
</commit_message>
<xml_diff>
--- a/doc/exposure_time.xlsx
+++ b/doc/exposure_time.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="360">
   <si>
     <t>0xFFFF</t>
   </si>
@@ -1094,9 +1094,6 @@
   </si>
   <si>
     <t>decimal value of the real value</t>
-  </si>
-  <si>
-    <t>x*16 = 200</t>
   </si>
 </sst>
 </file>
@@ -2394,11 +2391,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="165310400"/>
-        <c:axId val="165310976"/>
+        <c:axId val="166752192"/>
+        <c:axId val="166752768"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="165310400"/>
+        <c:axId val="166752192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2408,12 +2405,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="165310976"/>
+        <c:crossAx val="166752768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="165310976"/>
+        <c:axId val="166752768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2424,9 +2421,449 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="165310400"/>
+        <c:crossAx val="166752192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>exposition_time.xls!$E$2:$E$114</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="113"/>
+                <c:pt idx="0">
+                  <c:v>1050</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>866</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>833</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>666</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>633</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>566</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>533</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>466</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>433</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>366</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>333</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>283</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>266</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>233</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>216</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>187</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>173</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>9.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>8.6</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>7.3</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>6.6</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>5.6</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>5.3</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>4.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>4.3</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>3.3</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>1.35</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>1.1499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.93</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.86</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.73</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.66</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>0.53</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>0.46</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>0.43</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>0.33</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>0.23</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>0.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="129314304"/>
+        <c:axId val="129875264"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="129314304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="129875264"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="129875264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="129314304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2473,6 +2910,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Диаграмма 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2768,10 +3235,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L115"/>
+  <dimension ref="A1:F114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E114" sqref="E2:E114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5136,7 +5603,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>350</v>
       </c>
@@ -5157,7 +5624,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>352</v>
       </c>
@@ -5176,11 +5643,6 @@
       <c r="F114">
         <f t="shared" si="1"/>
         <v>13</v>
-      </c>
-    </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L115" t="s">
-        <v>360</v>
       </c>
     </row>
   </sheetData>

</xml_diff>